<commit_message>
Added print of stats in notebook
</commit_message>
<xml_diff>
--- a/PythonSourceCode/AirHeaterFMUWithPID/datafiles/describeExport.xlsx
+++ b/PythonSourceCode/AirHeaterFMUWithPID/datafiles/describeExport.xlsx
@@ -496,17 +496,17 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>controlSignal</t>
+          <t>controlSignalOME</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>outputTemperature</t>
+          <t>outputTemperatureOME</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>ambienteTemperature</t>
+          <t>ambienteTemperatureOME</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">

</xml_diff>